<commit_message>
Reviews for C, M, Z, OBI vplans
Signed-off-by: Arjan Bink <Arjan.Bink@silabs.com>
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_RV32C_Extension_Instructions.xlsx
+++ b/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_RV32C_Extension_Instructions.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\openhw\docs\core-v-docs.ArjanB_vplan_review\verif\CV32E40P\VerificationPlan\base_instruction_set\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1323DB4F-94D2-4993-ACAF-9E9C6B0BF936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="16380" windowHeight="8136" tabRatio="500"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RV32C" sheetId="1" r:id="rId1"/>
@@ -19,12 +25,13 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>GRASSET Arnaud</author>
+    <author>Arjan Bink</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -48,7 +55,62 @@
         </r>
       </text>
     </comment>
-    <comment ref="H4" authorId="0">
+    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{3A8381A2-50D0-40F8-AE8F-DF4CE634CE5C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Arjan Bink:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Check illegal instruction exception for c.ldsp, c.lqsp, c.fldsp
+Check illegal instruction exception for c.flwsp with F = 0
+Check illegal instruction exception for c.sdsp, c.sqsp, c.fsdsp
+Check illegal instruction exception for c.fswsp with F = 0
+Check illegal instruction exception for c.ld, c.lq, c.fld
+Check illegal instruction exception for c.flw with F = 0
+Check illegal instruction exception for reserved c.lwsp, c.flwsp encodings
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C4" authorId="1" shapeId="0" xr:uid="{53E00E3B-B9AE-49F8-9C08-AE7BDCE0FFD4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Arjan Bink:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Check that it is treated as illegal (only) if FPU=0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -72,7 +134,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -96,7 +158,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C7" authorId="0">
+    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -116,11 +178,108 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-TO BE CONFIRMED - F extension marked as tentative - 15/01/2020</t>
+TO BE CONFIRMED - F extension marked as tentative - 15/01/2020
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="A38" authorId="0">
+    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{0C1E44EF-A358-4312-9FE1-D9807001B273}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Arjan Bink:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Check that it is treated as illegal (only) if FPU=0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C10" authorId="1" shapeId="0" xr:uid="{AB751A0F-23D4-4C6C-9409-ADAF6523FF36}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Arjan Bink:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Check that it is treated as illegal (only) if FPU=0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C13" authorId="1" shapeId="0" xr:uid="{2D78EBE7-8A6E-4A19-A4A0-DD4DD95E54AD}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Arjan Bink:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Check that it is treated as illegal (only) if FPU=0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A21" authorId="1" shapeId="0" xr:uid="{AA237DFF-611B-4687-AFAD-4B94586088F3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Arjan Bink:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Check behavior of 'defined illegal instruction'</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="A38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -140,7 +299,8 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Do we support atomic extension ? This point should be part of the verification plan of the atomic extension ?</t>
+Do we support atomic extension ? This point should be part of the verification plan of the atomic extension ?
+Arjan Bink: No, we do not support 'A'</t>
         </r>
       </text>
     </comment>
@@ -2256,8 +2416,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="12">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2322,6 +2482,19 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -2453,6 +2626,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -2470,15 +2652,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2558,12 +2731,19 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2605,7 +2785,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2638,9 +2818,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2673,6 +2870,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2848,30 +3062,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D43" sqref="D43"/>
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.21875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="20.21875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="51.21875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="41.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5546875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.33203125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="35.33203125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="54.5546875" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="51.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="41.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="34.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.28515625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="54.5703125" style="1" customWidth="1"/>
     <col min="10" max="1023" width="17" style="1" customWidth="1"/>
-    <col min="1024" max="1025" width="9.109375" style="1" customWidth="1"/>
+    <col min="1024" max="1025" width="9.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1">
+    <row r="1" spans="1:9" s="4" customFormat="1" ht="30">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -2900,7 +3114,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="8" customFormat="1" ht="69">
+    <row r="2" spans="1:9" s="8" customFormat="1" ht="85.5">
       <c r="A2" s="7" t="s">
         <v>19</v>
       </c>
@@ -2925,11 +3139,11 @@
       </c>
       <c r="I2" s="5"/>
     </row>
-    <row r="3" spans="1:9" s="8" customFormat="1" ht="151.19999999999999" customHeight="1">
-      <c r="A3" s="33" t="s">
+    <row r="3" spans="1:9" s="8" customFormat="1" ht="151.15" customHeight="1">
+      <c r="A3" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="35" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -2952,9 +3166,9 @@
       </c>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" s="8" customFormat="1" ht="110.4">
-      <c r="A4" s="33"/>
-      <c r="B4" s="32"/>
+    <row r="4" spans="1:9" s="8" customFormat="1" ht="114">
+      <c r="A4" s="36"/>
+      <c r="B4" s="35"/>
       <c r="C4" s="24" t="s">
         <v>59</v>
       </c>
@@ -2975,32 +3189,32 @@
       </c>
       <c r="I4" s="26"/>
     </row>
-    <row r="5" spans="1:9" s="8" customFormat="1" ht="110.4">
-      <c r="A5" s="33"/>
-      <c r="B5" s="32"/>
-      <c r="C5" s="36" t="s">
+    <row r="5" spans="1:9" s="8" customFormat="1" ht="114">
+      <c r="A5" s="36"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="D5" s="36" t="s">
+      <c r="D5" s="30" t="s">
         <v>97</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="30" t="s">
         <v>119</v>
       </c>
-      <c r="F5" s="37" t="s">
+      <c r="F5" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="38"/>
-    </row>
-    <row r="6" spans="1:9" s="8" customFormat="1" ht="138">
-      <c r="A6" s="33"/>
-      <c r="B6" s="32"/>
+      <c r="I5" s="32"/>
+    </row>
+    <row r="6" spans="1:9" s="8" customFormat="1" ht="142.5">
+      <c r="A6" s="36"/>
+      <c r="B6" s="35"/>
       <c r="C6" s="6" t="s">
         <v>26</v>
       </c>
@@ -3021,9 +3235,9 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" s="8" customFormat="1" ht="138">
-      <c r="A7" s="33"/>
-      <c r="B7" s="32"/>
+    <row r="7" spans="1:9" s="8" customFormat="1" ht="142.5">
+      <c r="A7" s="36"/>
+      <c r="B7" s="35"/>
       <c r="C7" s="24" t="s">
         <v>60</v>
       </c>
@@ -3044,32 +3258,32 @@
       </c>
       <c r="I7" s="26"/>
     </row>
-    <row r="8" spans="1:9" s="8" customFormat="1" ht="138">
-      <c r="A8" s="33"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="36" t="s">
+    <row r="8" spans="1:9" s="8" customFormat="1" ht="142.5">
+      <c r="A8" s="36"/>
+      <c r="B8" s="35"/>
+      <c r="C8" s="30" t="s">
         <v>61</v>
       </c>
-      <c r="D8" s="36" t="s">
+      <c r="D8" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="F8" s="37" t="s">
+      <c r="F8" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="G8" s="36" t="s">
+      <c r="G8" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="37" t="s">
+      <c r="H8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="38"/>
-    </row>
-    <row r="9" spans="1:9" s="8" customFormat="1" ht="138">
-      <c r="A9" s="33"/>
-      <c r="B9" s="32"/>
+      <c r="I8" s="32"/>
+    </row>
+    <row r="9" spans="1:9" s="8" customFormat="1" ht="142.5">
+      <c r="A9" s="36"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="6" t="s">
         <v>27</v>
       </c>
@@ -3090,9 +3304,9 @@
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" s="8" customFormat="1" ht="110.4">
-      <c r="A10" s="33"/>
-      <c r="B10" s="32"/>
+    <row r="10" spans="1:9" s="8" customFormat="1" ht="114">
+      <c r="A10" s="36"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="24" t="s">
         <v>104</v>
       </c>
@@ -3113,32 +3327,32 @@
       </c>
       <c r="I10" s="5"/>
     </row>
-    <row r="11" spans="1:9" s="8" customFormat="1" ht="110.4">
-      <c r="A11" s="33"/>
-      <c r="B11" s="32"/>
-      <c r="C11" s="36" t="s">
+    <row r="11" spans="1:9" s="8" customFormat="1" ht="114">
+      <c r="A11" s="36"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="D11" s="36" t="s">
+      <c r="D11" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="30" t="s">
         <v>123</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="36" t="s">
+      <c r="G11" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="31" t="s">
         <v>12</v>
       </c>
       <c r="I11" s="5"/>
     </row>
-    <row r="12" spans="1:9" s="8" customFormat="1" ht="138">
-      <c r="A12" s="33"/>
-      <c r="B12" s="32"/>
+    <row r="12" spans="1:9" s="8" customFormat="1" ht="142.5">
+      <c r="A12" s="36"/>
+      <c r="B12" s="35"/>
       <c r="C12" s="6" t="s">
         <v>28</v>
       </c>
@@ -3159,9 +3373,9 @@
       </c>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" s="8" customFormat="1" ht="138">
-      <c r="A13" s="33"/>
-      <c r="B13" s="32"/>
+    <row r="13" spans="1:9" s="8" customFormat="1" ht="142.5">
+      <c r="A13" s="36"/>
+      <c r="B13" s="35"/>
       <c r="C13" s="24" t="s">
         <v>107</v>
       </c>
@@ -3182,34 +3396,34 @@
       </c>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" s="8" customFormat="1" ht="138">
-      <c r="A14" s="33"/>
-      <c r="B14" s="32"/>
-      <c r="C14" s="36" t="s">
+    <row r="14" spans="1:9" s="8" customFormat="1" ht="142.5">
+      <c r="A14" s="36"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="D14" s="36" t="s">
+      <c r="D14" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="31" t="s">
         <v>70</v>
       </c>
-      <c r="G14" s="36" t="s">
+      <c r="G14" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="31" t="s">
         <v>12</v>
       </c>
       <c r="I14" s="5"/>
     </row>
-    <row r="15" spans="1:9" s="8" customFormat="1" ht="69">
-      <c r="A15" s="33" t="s">
+    <row r="15" spans="1:9" s="8" customFormat="1" ht="71.25">
+      <c r="A15" s="36" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="35" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -3221,7 +3435,7 @@
       <c r="E15" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="33" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="17" t="s">
@@ -3232,9 +3446,9 @@
       </c>
       <c r="I15" s="5"/>
     </row>
-    <row r="16" spans="1:9" s="8" customFormat="1" ht="69">
-      <c r="A16" s="33"/>
-      <c r="B16" s="32"/>
+    <row r="16" spans="1:9" s="8" customFormat="1" ht="71.25">
+      <c r="A16" s="36"/>
+      <c r="B16" s="35"/>
       <c r="C16" s="6" t="s">
         <v>30</v>
       </c>
@@ -3244,7 +3458,7 @@
       <c r="E16" s="17" t="s">
         <v>126</v>
       </c>
-      <c r="F16" s="30"/>
+      <c r="F16" s="33"/>
       <c r="G16" s="17" t="s">
         <v>11</v>
       </c>
@@ -3253,9 +3467,9 @@
       </c>
       <c r="I16" s="5"/>
     </row>
-    <row r="17" spans="1:9" s="8" customFormat="1" ht="124.2">
-      <c r="A17" s="33"/>
-      <c r="B17" s="32"/>
+    <row r="17" spans="1:9" s="8" customFormat="1" ht="128.25">
+      <c r="A17" s="36"/>
+      <c r="B17" s="35"/>
       <c r="C17" s="6" t="s">
         <v>33</v>
       </c>
@@ -3276,9 +3490,9 @@
       </c>
       <c r="I17" s="5"/>
     </row>
-    <row r="18" spans="1:9" s="8" customFormat="1" ht="124.2">
-      <c r="A18" s="33"/>
-      <c r="B18" s="32"/>
+    <row r="18" spans="1:9" s="8" customFormat="1" ht="128.25">
+      <c r="A18" s="36"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="6" t="s">
         <v>34</v>
       </c>
@@ -3299,9 +3513,9 @@
       </c>
       <c r="I18" s="5"/>
     </row>
-    <row r="19" spans="1:9" s="8" customFormat="1" ht="138">
-      <c r="A19" s="33"/>
-      <c r="B19" s="32"/>
+    <row r="19" spans="1:9" s="8" customFormat="1" ht="142.5">
+      <c r="A19" s="36"/>
+      <c r="B19" s="35"/>
       <c r="C19" s="6" t="s">
         <v>35</v>
       </c>
@@ -3322,9 +3536,9 @@
       </c>
       <c r="I19" s="5"/>
     </row>
-    <row r="20" spans="1:9" s="8" customFormat="1" ht="138">
-      <c r="A20" s="33"/>
-      <c r="B20" s="32"/>
+    <row r="20" spans="1:9" s="8" customFormat="1" ht="142.5">
+      <c r="A20" s="36"/>
+      <c r="B20" s="35"/>
       <c r="C20" s="6" t="s">
         <v>36</v>
       </c>
@@ -3345,11 +3559,11 @@
       </c>
       <c r="I20" s="5"/>
     </row>
-    <row r="21" spans="1:9" s="8" customFormat="1" ht="110.4">
-      <c r="A21" s="33" t="s">
+    <row r="21" spans="1:9" s="8" customFormat="1" ht="114">
+      <c r="A21" s="36" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="35" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -3372,9 +3586,9 @@
       </c>
       <c r="I21" s="5"/>
     </row>
-    <row r="22" spans="1:9" s="8" customFormat="1" ht="110.4">
-      <c r="A22" s="33"/>
-      <c r="B22" s="32"/>
+    <row r="22" spans="1:9" s="8" customFormat="1" ht="114">
+      <c r="A22" s="36"/>
+      <c r="B22" s="35"/>
       <c r="C22" s="6" t="s">
         <v>39</v>
       </c>
@@ -3395,9 +3609,9 @@
       </c>
       <c r="I22" s="5"/>
     </row>
-    <row r="23" spans="1:9" s="8" customFormat="1" ht="138">
-      <c r="A23" s="33"/>
-      <c r="B23" s="32"/>
+    <row r="23" spans="1:9" s="8" customFormat="1" ht="142.5">
+      <c r="A23" s="36"/>
+      <c r="B23" s="35"/>
       <c r="C23" s="6" t="s">
         <v>40</v>
       </c>
@@ -3418,9 +3632,9 @@
       </c>
       <c r="I23" s="5"/>
     </row>
-    <row r="24" spans="1:9" s="8" customFormat="1" ht="96.6">
-      <c r="A24" s="33"/>
-      <c r="B24" s="32"/>
+    <row r="24" spans="1:9" s="8" customFormat="1" ht="99.75">
+      <c r="A24" s="36"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="6" t="s">
         <v>42</v>
       </c>
@@ -3441,9 +3655,9 @@
       </c>
       <c r="I24" s="5"/>
     </row>
-    <row r="25" spans="1:9" s="8" customFormat="1" ht="124.2">
-      <c r="A25" s="33"/>
-      <c r="B25" s="32"/>
+    <row r="25" spans="1:9" s="8" customFormat="1" ht="128.25">
+      <c r="A25" s="36"/>
+      <c r="B25" s="35"/>
       <c r="C25" s="6" t="s">
         <v>43</v>
       </c>
@@ -3464,9 +3678,9 @@
       </c>
       <c r="I25" s="5"/>
     </row>
-    <row r="26" spans="1:9" s="8" customFormat="1" ht="96.6">
-      <c r="A26" s="33"/>
-      <c r="B26" s="32"/>
+    <row r="26" spans="1:9" s="8" customFormat="1" ht="114">
+      <c r="A26" s="36"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="6" t="s">
         <v>44</v>
       </c>
@@ -3487,9 +3701,9 @@
       </c>
       <c r="I26" s="5"/>
     </row>
-    <row r="27" spans="1:9" s="8" customFormat="1" ht="96.6">
-      <c r="A27" s="33"/>
-      <c r="B27" s="32"/>
+    <row r="27" spans="1:9" s="8" customFormat="1" ht="114">
+      <c r="A27" s="36"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="6" t="s">
         <v>45</v>
       </c>
@@ -3510,9 +3724,9 @@
       </c>
       <c r="I27" s="5"/>
     </row>
-    <row r="28" spans="1:9" s="8" customFormat="1" ht="96.6">
-      <c r="A28" s="33"/>
-      <c r="B28" s="32"/>
+    <row r="28" spans="1:9" s="8" customFormat="1" ht="99.75">
+      <c r="A28" s="36"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="6" t="s">
         <v>46</v>
       </c>
@@ -3533,9 +3747,9 @@
       </c>
       <c r="I28" s="5"/>
     </row>
-    <row r="29" spans="1:9" s="8" customFormat="1" ht="124.2">
-      <c r="A29" s="33"/>
-      <c r="B29" s="32"/>
+    <row r="29" spans="1:9" s="8" customFormat="1" ht="128.25">
+      <c r="A29" s="36"/>
+      <c r="B29" s="35"/>
       <c r="C29" s="6" t="s">
         <v>57</v>
       </c>
@@ -3556,9 +3770,9 @@
       </c>
       <c r="I29" s="5"/>
     </row>
-    <row r="30" spans="1:9" s="8" customFormat="1" ht="69">
-      <c r="A30" s="33"/>
-      <c r="B30" s="32"/>
+    <row r="30" spans="1:9" s="8" customFormat="1" ht="85.5">
+      <c r="A30" s="36"/>
+      <c r="B30" s="35"/>
       <c r="C30" s="6" t="s">
         <v>47</v>
       </c>
@@ -3579,9 +3793,9 @@
       </c>
       <c r="I30" s="5"/>
     </row>
-    <row r="31" spans="1:9" s="8" customFormat="1" ht="110.4">
-      <c r="A31" s="33"/>
-      <c r="B31" s="32"/>
+    <row r="31" spans="1:9" s="8" customFormat="1" ht="114">
+      <c r="A31" s="36"/>
+      <c r="B31" s="35"/>
       <c r="C31" s="6" t="s">
         <v>48</v>
       </c>
@@ -3602,9 +3816,9 @@
       </c>
       <c r="I31" s="5"/>
     </row>
-    <row r="32" spans="1:9" s="8" customFormat="1" ht="96.6">
-      <c r="A32" s="33"/>
-      <c r="B32" s="32"/>
+    <row r="32" spans="1:9" s="8" customFormat="1" ht="99.75">
+      <c r="A32" s="36"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="6" t="s">
         <v>49</v>
       </c>
@@ -3625,9 +3839,9 @@
       </c>
       <c r="I32" s="5"/>
     </row>
-    <row r="33" spans="1:9" s="8" customFormat="1" ht="96.6">
-      <c r="A33" s="33"/>
-      <c r="B33" s="32"/>
+    <row r="33" spans="1:9" s="8" customFormat="1" ht="99.75">
+      <c r="A33" s="36"/>
+      <c r="B33" s="35"/>
       <c r="C33" s="6" t="s">
         <v>50</v>
       </c>
@@ -3648,9 +3862,9 @@
       </c>
       <c r="I33" s="5"/>
     </row>
-    <row r="34" spans="1:9" s="8" customFormat="1" ht="96.6">
-      <c r="A34" s="33"/>
-      <c r="B34" s="32"/>
+    <row r="34" spans="1:9" s="8" customFormat="1" ht="99.75">
+      <c r="A34" s="36"/>
+      <c r="B34" s="35"/>
       <c r="C34" s="6" t="s">
         <v>51</v>
       </c>
@@ -3671,9 +3885,9 @@
       </c>
       <c r="I34" s="5"/>
     </row>
-    <row r="35" spans="1:9" s="8" customFormat="1" ht="96.6">
-      <c r="A35" s="33"/>
-      <c r="B35" s="32"/>
+    <row r="35" spans="1:9" s="8" customFormat="1" ht="114">
+      <c r="A35" s="36"/>
+      <c r="B35" s="35"/>
       <c r="C35" s="6" t="s">
         <v>52</v>
       </c>
@@ -3694,9 +3908,9 @@
       </c>
       <c r="I35" s="5"/>
     </row>
-    <row r="36" spans="1:9" s="8" customFormat="1" ht="41.4">
-      <c r="A36" s="33"/>
-      <c r="B36" s="32"/>
+    <row r="36" spans="1:9" s="8" customFormat="1" ht="42.75">
+      <c r="A36" s="36"/>
+      <c r="B36" s="35"/>
       <c r="C36" s="6" t="s">
         <v>53</v>
       </c>
@@ -3717,9 +3931,9 @@
       </c>
       <c r="I36" s="5"/>
     </row>
-    <row r="37" spans="1:9" s="8" customFormat="1" ht="42.6">
-      <c r="A37" s="33"/>
-      <c r="B37" s="32"/>
+    <row r="37" spans="1:9" s="8" customFormat="1" ht="44.25">
+      <c r="A37" s="36"/>
+      <c r="B37" s="35"/>
       <c r="C37" s="6" t="s">
         <v>54</v>
       </c>
@@ -3734,7 +3948,7 @@
       <c r="H37" s="23"/>
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="1:9" s="8" customFormat="1" ht="69">
+    <row r="38" spans="1:9" s="8" customFormat="1" ht="71.25">
       <c r="A38" s="12" t="s">
         <v>55</v>
       </c>
@@ -3750,10 +3964,10 @@
       <c r="I38" s="5"/>
     </row>
     <row r="39" spans="1:9" s="8" customFormat="1" ht="18" customHeight="1">
-      <c r="A39" s="33" t="s">
+      <c r="A39" s="36" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="32" t="s">
+      <c r="B39" s="35" t="s">
         <v>85</v>
       </c>
       <c r="C39" s="6" t="s">
@@ -3762,167 +3976,167 @@
       <c r="D39" s="28" t="s">
         <v>90</v>
       </c>
-      <c r="E39" s="32" t="s">
+      <c r="E39" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="F39" s="34" t="s">
+      <c r="F39" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="34" t="s">
+      <c r="G39" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="H39" s="35" t="s">
+      <c r="H39" s="38" t="s">
         <v>17</v>
       </c>
       <c r="I39" s="5"/>
     </row>
     <row r="40" spans="1:9" s="8" customFormat="1">
-      <c r="A40" s="33"/>
-      <c r="B40" s="32"/>
+      <c r="A40" s="36"/>
+      <c r="B40" s="35"/>
       <c r="C40" s="27" t="s">
         <v>40</v>
       </c>
       <c r="D40" s="28" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="32"/>
-      <c r="F40" s="34"/>
-      <c r="G40" s="34"/>
-      <c r="H40" s="35"/>
+      <c r="E40" s="35"/>
+      <c r="F40" s="37"/>
+      <c r="G40" s="37"/>
+      <c r="H40" s="38"/>
       <c r="I40" s="5"/>
     </row>
     <row r="41" spans="1:9" s="8" customFormat="1">
-      <c r="A41" s="33"/>
-      <c r="B41" s="32"/>
+      <c r="A41" s="36"/>
+      <c r="B41" s="35"/>
       <c r="C41" s="27" t="s">
         <v>38</v>
       </c>
       <c r="D41" s="28" t="s">
         <v>92</v>
       </c>
-      <c r="E41" s="32"/>
-      <c r="F41" s="34"/>
-      <c r="G41" s="34"/>
-      <c r="H41" s="35"/>
+      <c r="E41" s="35"/>
+      <c r="F41" s="37"/>
+      <c r="G41" s="37"/>
+      <c r="H41" s="38"/>
       <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:9" s="8" customFormat="1">
-      <c r="A42" s="33"/>
-      <c r="B42" s="32"/>
+      <c r="A42" s="36"/>
+      <c r="B42" s="35"/>
       <c r="C42" s="27" t="s">
         <v>39</v>
       </c>
       <c r="D42" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="32"/>
-      <c r="F42" s="34"/>
-      <c r="G42" s="34"/>
-      <c r="H42" s="35"/>
+      <c r="E42" s="35"/>
+      <c r="F42" s="37"/>
+      <c r="G42" s="37"/>
+      <c r="H42" s="38"/>
       <c r="I42" s="5"/>
     </row>
     <row r="43" spans="1:9" s="8" customFormat="1">
-      <c r="A43" s="33"/>
-      <c r="B43" s="32"/>
+      <c r="A43" s="36"/>
+      <c r="B43" s="35"/>
       <c r="C43" s="27" t="s">
         <v>47</v>
       </c>
       <c r="D43" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="32"/>
-      <c r="F43" s="34"/>
-      <c r="G43" s="34"/>
-      <c r="H43" s="35"/>
+      <c r="E43" s="35"/>
+      <c r="F43" s="37"/>
+      <c r="G43" s="37"/>
+      <c r="H43" s="38"/>
       <c r="I43" s="5"/>
     </row>
     <row r="44" spans="1:9" s="8" customFormat="1">
-      <c r="A44" s="33"/>
-      <c r="B44" s="32"/>
+      <c r="A44" s="36"/>
+      <c r="B44" s="35"/>
       <c r="C44" s="27" t="s">
         <v>48</v>
       </c>
       <c r="D44" s="28" t="s">
         <v>94</v>
       </c>
-      <c r="E44" s="32"/>
-      <c r="F44" s="34"/>
-      <c r="G44" s="34"/>
-      <c r="H44" s="35"/>
+      <c r="E44" s="35"/>
+      <c r="F44" s="37"/>
+      <c r="G44" s="37"/>
+      <c r="H44" s="38"/>
       <c r="I44" s="5"/>
     </row>
     <row r="45" spans="1:9" s="8" customFormat="1">
-      <c r="A45" s="33"/>
-      <c r="B45" s="32"/>
+      <c r="A45" s="36"/>
+      <c r="B45" s="35"/>
       <c r="C45" s="27" t="s">
         <v>44</v>
       </c>
       <c r="D45" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="E45" s="32"/>
-      <c r="F45" s="34"/>
-      <c r="G45" s="34"/>
-      <c r="H45" s="35"/>
+      <c r="E45" s="35"/>
+      <c r="F45" s="37"/>
+      <c r="G45" s="37"/>
+      <c r="H45" s="38"/>
       <c r="I45" s="5"/>
     </row>
     <row r="46" spans="1:9" s="8" customFormat="1">
-      <c r="A46" s="33"/>
-      <c r="B46" s="32"/>
+      <c r="A46" s="36"/>
+      <c r="B46" s="35"/>
       <c r="C46" s="27" t="s">
         <v>86</v>
       </c>
       <c r="D46" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="32"/>
-      <c r="F46" s="34"/>
-      <c r="G46" s="34"/>
-      <c r="H46" s="35"/>
+      <c r="E46" s="35"/>
+      <c r="F46" s="37"/>
+      <c r="G46" s="37"/>
+      <c r="H46" s="38"/>
       <c r="I46" s="5"/>
     </row>
     <row r="47" spans="1:9" s="8" customFormat="1">
-      <c r="A47" s="33"/>
-      <c r="B47" s="32"/>
+      <c r="A47" s="36"/>
+      <c r="B47" s="35"/>
       <c r="C47" s="27" t="s">
         <v>87</v>
       </c>
       <c r="D47" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="32"/>
-      <c r="F47" s="34"/>
-      <c r="G47" s="34"/>
-      <c r="H47" s="35"/>
+      <c r="E47" s="35"/>
+      <c r="F47" s="37"/>
+      <c r="G47" s="37"/>
+      <c r="H47" s="38"/>
       <c r="I47" s="5"/>
     </row>
     <row r="48" spans="1:9" s="8" customFormat="1">
-      <c r="A48" s="33"/>
-      <c r="B48" s="32"/>
+      <c r="A48" s="36"/>
+      <c r="B48" s="35"/>
       <c r="C48" s="27" t="s">
         <v>88</v>
       </c>
       <c r="D48" s="28" t="s">
         <v>95</v>
       </c>
-      <c r="E48" s="32"/>
-      <c r="F48" s="34"/>
-      <c r="G48" s="34"/>
-      <c r="H48" s="35"/>
+      <c r="E48" s="35"/>
+      <c r="F48" s="37"/>
+      <c r="G48" s="37"/>
+      <c r="H48" s="38"/>
       <c r="I48" s="5"/>
     </row>
     <row r="49" spans="1:9" s="10" customFormat="1">
-      <c r="A49" s="31" t="s">
+      <c r="A49" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="31"/>
-      <c r="C49" s="31"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="31"/>
-      <c r="G49" s="31"/>
-      <c r="H49" s="31"/>
-      <c r="I49" s="31"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="34"/>
+      <c r="D49" s="34"/>
+      <c r="E49" s="34"/>
+      <c r="F49" s="34"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="34"/>
+      <c r="I49" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>

<commit_message>
Responded to review comments
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_RV32C_Extension_Instructions.xlsx
+++ b/verif/CV32E40P/VerificationPlan/base_instruction_set/CV32E40P_RV32C_Extension_Instructions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\openhw\docs\core-v-docs.ArjanB_vplan_review\verif\CV32E40P\VerificationPlan\base_instruction_set\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1323DB4F-94D2-4993-ACAF-9E9C6B0BF936}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D31464E-6253-4684-BC1A-DD4D80E91138}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RV32C" sheetId="1" r:id="rId1"/>
@@ -27,55 +27,35 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
-    <author>GRASSET Arnaud</author>
-    <author>Arjan Bink</author>
+    <author>tc={4633BBA7-FFAF-4E47-AB82-D190A1C619E2}</author>
+    <author>tc={C79E9168-4D6E-406D-841C-F25BB2A98DD0}</author>
+    <author>tc={70488D3D-F3E0-47A8-ABC6-90CE63F82DA1}</author>
+    <author>tc={96B9FCB9-2E29-4198-AC4E-DBFF99F13FCA}</author>
+    <author>tc={0DCA8A89-A291-4ACC-BF92-379B0D24E9EC}</author>
+    <author>tc={B18D8C48-3A7F-4D26-8C4B-592ECE9409AF}</author>
+    <author>tc={4FAD508D-AE90-4955-9E31-03DB237427D8}</author>
+    <author>tc={03EB4278-BE6D-42EA-B589-157D52AEC6A0}</author>
+    <author>tc={B1BCC209-E6EB-4987-AE24-B12D05A04BED}</author>
+    <author>tc={8E23BB49-38EC-470A-949C-4C9BA05B0675}</author>
+    <author>tc={3A22FB71-F33F-43F1-8516-FAB9A1D90679}</author>
   </authors>
   <commentList>
-    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{4633BBA7-FFAF-4E47-AB82-D190A1C619E2}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>GRASSET Arnaud:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Remove test of instruction-address-misaligned from CV32E40P_instruction_exceptions.xlsx?</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Remove test of instruction-address-misaligned from CV32E40P_instruction_exceptions.xlsx?
+Reply:
+    Yes, that was removed from the Exceptions Vplan as the CV32E40P will not attempt to fetch from byte boundaries and byte aligned instructions are indistinquishable from illegal instructions.</t>
       </text>
     </comment>
-    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{3A8381A2-50D0-40F8-AE8F-DF4CE634CE5C}">
+    <comment ref="B3" authorId="1" shapeId="0" xr:uid="{C79E9168-4D6E-406D-841C-F25BB2A98DD0}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Arjan Bink:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Check illegal instruction exception for c.ldsp, c.lqsp, c.fldsp
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Check illegal instruction exception for c.ldsp, c.lqsp, c.fldsp
 Check illegal instruction exception for c.flwsp with F = 0
 Check illegal instruction exception for c.sdsp, c.sqsp, c.fsdsp
 Check illegal instruction exception for c.fswsp with F = 0
@@ -83,225 +63,95 @@
 Check illegal instruction exception for c.flw with F = 0
 Check illegal instruction exception for reserved c.lwsp, c.flwsp encodings
 </t>
-        </r>
       </text>
     </comment>
-    <comment ref="C4" authorId="1" shapeId="0" xr:uid="{53E00E3B-B9AE-49F8-9C08-AE7BDCE0FFD4}">
+    <comment ref="C4" authorId="2" shapeId="0" xr:uid="{70488D3D-F3E0-47A8-ABC6-90CE63F82DA1}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Arjan Bink:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Check that it is treated as illegal (only) if FPU=0</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Check that it is treated as illegal (only) if FPU=0
+Reply:
+    Done.  In fact, for CV32E40P we will only test with FPU=0.</t>
       </text>
     </comment>
-    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
+    <comment ref="H4" authorId="3" shapeId="0" xr:uid="{96B9FCB9-2E29-4198-AC4E-DBFF99F13FCA}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>GRASSET Arnaud:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-TO BE CONFIRMED - F extension marked as tentative - 15/01/2020</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    TO BE CONFIRMED - F extension marked as tentative - 15/01/2020
+Reply:
+    CV32E40P will be verified with FPU=0</t>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
+    <comment ref="C5" authorId="4" shapeId="0" xr:uid="{0DCA8A89-A291-4ACC-BF92-379B0D24E9EC}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>GRASSET Arnaud:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-TO DELETE - D extension not supported</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    TO DELETE - D extension not supported
+Reply:
+    Yes, you are right.  This could be deleted, or we could check to see that it is recognized as an illegal instruction (overkill?).</t>
       </text>
     </comment>
-    <comment ref="C7" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
+    <comment ref="C7" authorId="5" shapeId="0" xr:uid="{B18D8C48-3A7F-4D26-8C4B-592ECE9409AF}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>GRASSET Arnaud:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-TO BE CONFIRMED - F extension marked as tentative - 15/01/2020
-</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    TO BE CONFIRMED - F extension marked as tentative - 15/01/2020
+Reply:
+    CV32E40P will be verified with FPU=0 only</t>
       </text>
     </comment>
-    <comment ref="D7" authorId="1" shapeId="0" xr:uid="{0C1E44EF-A358-4312-9FE1-D9807001B273}">
+    <comment ref="D7" authorId="6" shapeId="0" xr:uid="{4FAD508D-AE90-4955-9E31-03DB237427D8}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Arjan Bink:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Check that it is treated as illegal (only) if FPU=0</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Check that it is treated as illegal (only) if FPU=0
+Reply:
+    Updated for illegal instruction</t>
       </text>
     </comment>
-    <comment ref="C10" authorId="1" shapeId="0" xr:uid="{AB751A0F-23D4-4C6C-9409-ADAF6523FF36}">
+    <comment ref="C10" authorId="7" shapeId="0" xr:uid="{03EB4278-BE6D-42EA-B589-157D52AEC6A0}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Arjan Bink:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Check that it is treated as illegal (only) if FPU=0</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Check that it is treated as illegal (only) if FPU=0
+Reply:
+    Updated for illegal instruction</t>
       </text>
     </comment>
-    <comment ref="C13" authorId="1" shapeId="0" xr:uid="{2D78EBE7-8A6E-4A19-A4A0-DD4DD95E54AD}">
+    <comment ref="C13" authorId="8" shapeId="0" xr:uid="{B1BCC209-E6EB-4987-AE24-B12D05A04BED}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Arjan Bink:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Check that it is treated as illegal (only) if FPU=0</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Check that it is treated as illegal (only) if FPU=0
+Reply:
+    Updated for illegal instruction</t>
       </text>
     </comment>
-    <comment ref="A21" authorId="1" shapeId="0" xr:uid="{AA237DFF-611B-4687-AFAD-4B94586088F3}">
+    <comment ref="A21" authorId="9" shapeId="0" xr:uid="{8E23BB49-38EC-470A-949C-4C9BA05B0675}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Arjan Bink:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-Check behavior of 'defined illegal instruction'</t>
-        </r>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Check behavior of 'defined illegal instruction'
+Reply:
+    Done.  Thanks!</t>
       </text>
     </comment>
-    <comment ref="A38" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
+    <comment ref="A39" authorId="10" shapeId="0" xr:uid="{3A22FB71-F33F-43F1-8516-FAB9A1D90679}">
       <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>GRASSET Arnaud:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Do we support atomic extension ? This point should be part of the verification plan of the atomic extension ?
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Do we support atomic extension ? This point should be part of the verification plan of the atomic extension ?
 Arjan Bink: No, we do not support 'A'</t>
-        </r>
       </text>
     </comment>
   </commentList>
@@ -309,7 +159,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="257" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="152">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -2300,11 +2150,6 @@
 No need for exhaustive coverage of all immediate and registers values</t>
   </si>
   <si>
-    <t>Exercise instruction using all legal destination floating-point registers.
-Cover different values of uimm, including minimum and maximum values.
-No need for exhaustive coverage of all immediate and registers values</t>
-  </si>
-  <si>
     <t>Memory written with expected values.
 Exercise instruction using all legal source GPRs.
 Cover different values of uimm, including minimum and maximum values.
@@ -2411,13 +2256,420 @@
     <t>Exercise instruction using all combinations of source and destination operands (x8-x15).
 Exercise underflow.
 No need for exhaustive coverage of all immediate and registers values</t>
+  </si>
+  <si>
+    <t>Treated as illegal instruction when FPU=0</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Pass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: c.flwsp is fetched and an illegal instruction exception occurs.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Fail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">:  c.flwsp is fetched and an illegal instruction exception </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">does not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>occur.</t>
+    </r>
+  </si>
+  <si>
+    <t>Directed Test</t>
+  </si>
+  <si>
+    <t>Test case.
+No specific functional coverage.</t>
+  </si>
+  <si>
+    <t>Treated as illegal instruction (regardless of FPU value)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Pass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: c.fldsp is fetched and an illegal instruction exception occurs.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Fail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">:  c.fldsp is fetched and an illegal instruction exception </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">does not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>occur.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Pass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: c.fswsp is fetched and an illegal instruction exception occurs.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Fail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">:  c.fswsp is fetched and an illegal instruction exception </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">does not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>occur.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Pass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: c.flw is fetched and an illegal instruction exception occurs.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Fail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">:  c.flw is fetched and an illegal instruction exception </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">does not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>occur.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Pass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: c.fsw is fetched and an illegal instruction exception occurs.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Fail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">:  c.fsw is fetched and an illegal instruction exception </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">does not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>occur.</t>
+    </r>
+  </si>
+  <si>
+    <t>Defined Illegal Instruction</t>
+  </si>
+  <si>
+    <t>A 16-bit instruction with all bits zero is an illegal instruction.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Pass</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t>: 16'h0000 is fetched and an illegal instruction exception occurs.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>Fail</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">:  16'h0000 is fetched and an illegal instruction exception </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t xml:space="preserve">does not </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="DejaVu Sans"/>
+      </rPr>
+      <t>occur.</t>
+    </r>
+  </si>
+  <si>
+    <t>Treated as illegal instruction (always)
+Test with both 32-bit and 16-bit alignment.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12">
+  <fonts count="11">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -2444,19 +2696,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="DejaVu Sans"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
       <family val="2"/>
     </font>
     <font>
@@ -2490,14 +2729,18 @@
       <charset val="1"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="DejaVu Sans"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2522,12 +2765,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -2541,7 +2778,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2612,9 +2849,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2626,14 +2860,14 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -2652,6 +2886,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2739,7 +2985,11 @@
 </file>
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Mike" id="{237EBA78-1434-4846-B3EF-5D4C944F8BB2}" userId="Mike" providerId="None"/>
+  <person displayName="Arjan Bink" id="{9C48A28D-C119-42E3-BE0E-74C2D3B4DFF6}" userId="Arjan Bink" providerId="None"/>
+  <person displayName="GRASSET Arnaud" id="{08D0BE41-6009-49B9-94CB-8A0FA3031169}" userId="GRASSET Arnaud" providerId="None"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3061,24 +3311,98 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="A2" personId="{08D0BE41-6009-49B9-94CB-8A0FA3031169}" id="{4633BBA7-FFAF-4E47-AB82-D190A1C619E2}">
+    <text>Remove test of instruction-address-misaligned from CV32E40P_instruction_exceptions.xlsx?</text>
+  </threadedComment>
+  <threadedComment ref="A2" dT="2020-09-17T18:44:49.91" personId="{237EBA78-1434-4846-B3EF-5D4C944F8BB2}" id="{C4DC78D5-AE50-4251-A647-D319F0B252F7}" parentId="{4633BBA7-FFAF-4E47-AB82-D190A1C619E2}">
+    <text>Yes, that was removed from the Exceptions Vplan as the CV32E40P will not attempt to fetch from byte boundaries and byte aligned instructions are indistinquishable from illegal instructions.</text>
+  </threadedComment>
+  <threadedComment ref="B3" personId="{9C48A28D-C119-42E3-BE0E-74C2D3B4DFF6}" id="{C79E9168-4D6E-406D-841C-F25BB2A98DD0}">
+    <text xml:space="preserve">Check illegal instruction exception for c.ldsp, c.lqsp, c.fldsp
+Check illegal instruction exception for c.flwsp with F = 0
+Check illegal instruction exception for c.sdsp, c.sqsp, c.fsdsp
+Check illegal instruction exception for c.fswsp with F = 0
+Check illegal instruction exception for c.ld, c.lq, c.fld
+Check illegal instruction exception for c.flw with F = 0
+Check illegal instruction exception for reserved c.lwsp, c.flwsp encodings
+</text>
+  </threadedComment>
+  <threadedComment ref="C4" personId="{9C48A28D-C119-42E3-BE0E-74C2D3B4DFF6}" id="{70488D3D-F3E0-47A8-ABC6-90CE63F82DA1}">
+    <text>Check that it is treated as illegal (only) if FPU=0</text>
+  </threadedComment>
+  <threadedComment ref="C4" dT="2020-09-17T18:55:24.56" personId="{237EBA78-1434-4846-B3EF-5D4C944F8BB2}" id="{8CE2DDBB-2085-4354-8AE6-3D03274AD6F7}" parentId="{70488D3D-F3E0-47A8-ABC6-90CE63F82DA1}">
+    <text>Done.  In fact, for CV32E40P we will only test with FPU=0.</text>
+  </threadedComment>
+  <threadedComment ref="H4" personId="{08D0BE41-6009-49B9-94CB-8A0FA3031169}" id="{96B9FCB9-2E29-4198-AC4E-DBFF99F13FCA}">
+    <text>TO BE CONFIRMED - F extension marked as tentative - 15/01/2020</text>
+  </threadedComment>
+  <threadedComment ref="H4" dT="2020-09-17T18:56:14.10" personId="{237EBA78-1434-4846-B3EF-5D4C944F8BB2}" id="{83643B02-B9E1-49E2-AA52-DB51EFA233FB}" parentId="{96B9FCB9-2E29-4198-AC4E-DBFF99F13FCA}">
+    <text>CV32E40P will be verified with FPU=0</text>
+  </threadedComment>
+  <threadedComment ref="C5" personId="{08D0BE41-6009-49B9-94CB-8A0FA3031169}" id="{0DCA8A89-A291-4ACC-BF92-379B0D24E9EC}">
+    <text>TO DELETE - D extension not supported</text>
+  </threadedComment>
+  <threadedComment ref="C5" dT="2020-09-17T18:58:57.32" personId="{237EBA78-1434-4846-B3EF-5D4C944F8BB2}" id="{46CEBA6E-B408-4FE2-8E69-0120797A01BD}" parentId="{0DCA8A89-A291-4ACC-BF92-379B0D24E9EC}">
+    <text>Yes, you are right.  This could be deleted, or we could check to see that it is recognized as an illegal instruction (overkill?).</text>
+  </threadedComment>
+  <threadedComment ref="C7" personId="{08D0BE41-6009-49B9-94CB-8A0FA3031169}" id="{B18D8C48-3A7F-4D26-8C4B-592ECE9409AF}">
+    <text xml:space="preserve">TO BE CONFIRMED - F extension marked as tentative - 15/01/2020
+</text>
+  </threadedComment>
+  <threadedComment ref="C7" dT="2020-09-17T18:59:56.78" personId="{237EBA78-1434-4846-B3EF-5D4C944F8BB2}" id="{E5B960BF-C820-4C7E-8C85-ED5CAEAE0DA6}" parentId="{B18D8C48-3A7F-4D26-8C4B-592ECE9409AF}">
+    <text>CV32E40P will be verified with FPU=0 only</text>
+  </threadedComment>
+  <threadedComment ref="D7" personId="{9C48A28D-C119-42E3-BE0E-74C2D3B4DFF6}" id="{4FAD508D-AE90-4955-9E31-03DB237427D8}">
+    <text>Check that it is treated as illegal (only) if FPU=0</text>
+  </threadedComment>
+  <threadedComment ref="D7" dT="2020-09-17T19:02:12.02" personId="{237EBA78-1434-4846-B3EF-5D4C944F8BB2}" id="{E335B8BA-235B-4F9A-9B03-DCFB33D8B020}" parentId="{4FAD508D-AE90-4955-9E31-03DB237427D8}">
+    <text>Updated for illegal instruction</text>
+  </threadedComment>
+  <threadedComment ref="C10" personId="{9C48A28D-C119-42E3-BE0E-74C2D3B4DFF6}" id="{03EB4278-BE6D-42EA-B589-157D52AEC6A0}">
+    <text>Check that it is treated as illegal (only) if FPU=0</text>
+  </threadedComment>
+  <threadedComment ref="C10" dT="2020-09-17T19:02:55.76" personId="{237EBA78-1434-4846-B3EF-5D4C944F8BB2}" id="{2762A40C-6C89-46BD-A1B6-A4FEB650199B}" parentId="{03EB4278-BE6D-42EA-B589-157D52AEC6A0}">
+    <text>Updated for illegal instruction</text>
+  </threadedComment>
+  <threadedComment ref="C13" personId="{9C48A28D-C119-42E3-BE0E-74C2D3B4DFF6}" id="{B1BCC209-E6EB-4987-AE24-B12D05A04BED}">
+    <text>Check that it is treated as illegal (only) if FPU=0</text>
+  </threadedComment>
+  <threadedComment ref="C13" dT="2020-09-17T19:04:35.71" personId="{237EBA78-1434-4846-B3EF-5D4C944F8BB2}" id="{3E88415B-A047-4F2C-B54D-63821E311183}" parentId="{B1BCC209-E6EB-4987-AE24-B12D05A04BED}">
+    <text>Updated for illegal instruction</text>
+  </threadedComment>
+  <threadedComment ref="A21" personId="{9C48A28D-C119-42E3-BE0E-74C2D3B4DFF6}" id="{8E23BB49-38EC-470A-949C-4C9BA05B0675}">
+    <text>Check behavior of 'defined illegal instruction'</text>
+  </threadedComment>
+  <threadedComment ref="A21" dT="2020-09-17T19:19:01.29" personId="{237EBA78-1434-4846-B3EF-5D4C944F8BB2}" id="{387E5439-C75C-4869-B376-301FACE91619}" parentId="{8E23BB49-38EC-470A-949C-4C9BA05B0675}">
+    <text>Done.  Thanks!</text>
+  </threadedComment>
+  <threadedComment ref="A39" personId="{08D0BE41-6009-49B9-94CB-8A0FA3031169}" id="{3A22FB71-F33F-43F1-8516-FAB9A1D90679}" done="1">
+    <text>Do we support atomic extension ? This point should be part of the verification plan of the atomic extension ?
+Arjan Bink: No, we do not support 'A'</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AMK49"/>
+  <dimension ref="A1:AMK50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="21.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="51.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="41.28515625" style="1" customWidth="1"/>
     <col min="6" max="6" width="34.5703125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="12.28515625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" style="1" customWidth="1"/>
     <col min="8" max="8" width="35.28515625" style="1" customWidth="1"/>
     <col min="9" max="9" width="54.5703125" style="1" customWidth="1"/>
     <col min="10" max="1023" width="17" style="1" customWidth="1"/>
@@ -3086,7 +3410,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="4" customFormat="1" ht="30">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="41" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -3140,10 +3464,10 @@
       <c r="I2" s="5"/>
     </row>
     <row r="3" spans="1:9" s="8" customFormat="1" ht="151.15" customHeight="1">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>24</v>
       </c>
       <c r="C3" s="6" t="s">
@@ -3166,32 +3490,32 @@
       </c>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" s="8" customFormat="1" ht="114">
-      <c r="A4" s="36"/>
-      <c r="B4" s="35"/>
-      <c r="C4" s="24" t="s">
+    <row r="4" spans="1:9" s="8" customFormat="1" ht="88.5">
+      <c r="A4" s="35"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="E4" s="24" t="s">
-        <v>119</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="I4" s="26"/>
-    </row>
-    <row r="5" spans="1:9" s="8" customFormat="1" ht="114">
-      <c r="A5" s="36"/>
-      <c r="B5" s="35"/>
+      <c r="E4" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F4" s="38" t="s">
+        <v>140</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="I4" s="39"/>
+    </row>
+    <row r="5" spans="1:9" s="8" customFormat="1" ht="88.5">
+      <c r="A5" s="35"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="30" t="s">
         <v>58</v>
       </c>
@@ -3199,22 +3523,22 @@
         <v>97</v>
       </c>
       <c r="E5" s="30" t="s">
-        <v>119</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>9</v>
+        <v>143</v>
+      </c>
+      <c r="F5" s="38" t="s">
+        <v>144</v>
       </c>
       <c r="G5" s="30" t="s">
-        <v>11</v>
+        <v>141</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>12</v>
-      </c>
-      <c r="I5" s="32"/>
+        <v>142</v>
+      </c>
+      <c r="I5" s="39"/>
     </row>
     <row r="6" spans="1:9" s="8" customFormat="1" ht="142.5">
-      <c r="A6" s="36"/>
-      <c r="B6" s="35"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="34"/>
       <c r="C6" s="6" t="s">
         <v>26</v>
       </c>
@@ -3222,7 +3546,7 @@
         <v>99</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F6" s="18" t="s">
         <v>70</v>
@@ -3235,32 +3559,32 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" s="8" customFormat="1" ht="142.5">
-      <c r="A7" s="36"/>
-      <c r="B7" s="35"/>
+    <row r="7" spans="1:9" s="8" customFormat="1" ht="88.5">
+      <c r="A7" s="35"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="24" t="s">
         <v>60</v>
       </c>
       <c r="D7" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="E7" s="24" t="s">
-        <v>121</v>
-      </c>
-      <c r="F7" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>12</v>
-      </c>
-      <c r="I7" s="26"/>
+      <c r="E7" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F7" s="38" t="s">
+        <v>145</v>
+      </c>
+      <c r="G7" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="H7" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="I7" s="25"/>
     </row>
     <row r="8" spans="1:9" s="8" customFormat="1" ht="142.5">
-      <c r="A8" s="36"/>
-      <c r="B8" s="35"/>
+      <c r="A8" s="35"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="30" t="s">
         <v>61</v>
       </c>
@@ -3268,7 +3592,7 @@
         <v>69</v>
       </c>
       <c r="E8" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F8" s="31" t="s">
         <v>70</v>
@@ -3279,11 +3603,11 @@
       <c r="H8" s="31" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="32"/>
+      <c r="I8" s="39"/>
     </row>
     <row r="9" spans="1:9" s="8" customFormat="1" ht="142.5">
-      <c r="A9" s="36"/>
-      <c r="B9" s="35"/>
+      <c r="A9" s="35"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="6" t="s">
         <v>27</v>
       </c>
@@ -3291,7 +3615,7 @@
         <v>100</v>
       </c>
       <c r="E9" s="13" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F9" s="18" t="s">
         <v>9</v>
@@ -3304,32 +3628,32 @@
       </c>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" s="8" customFormat="1" ht="114">
-      <c r="A10" s="36"/>
-      <c r="B10" s="35"/>
+    <row r="10" spans="1:9" s="8" customFormat="1" ht="87.75">
+      <c r="A10" s="35"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="24" t="s">
         <v>104</v>
       </c>
       <c r="D10" s="24" t="s">
         <v>102</v>
       </c>
-      <c r="E10" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="F10" s="25" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>12</v>
+      <c r="E10" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F10" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="H10" s="31" t="s">
+        <v>142</v>
       </c>
       <c r="I10" s="5"/>
     </row>
     <row r="11" spans="1:9" s="8" customFormat="1" ht="114">
-      <c r="A11" s="36"/>
-      <c r="B11" s="35"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="30" t="s">
         <v>105</v>
       </c>
@@ -3337,7 +3661,7 @@
         <v>103</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F11" s="31" t="s">
         <v>9</v>
@@ -3351,8 +3675,8 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" s="8" customFormat="1" ht="142.5">
-      <c r="A12" s="36"/>
-      <c r="B12" s="35"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="34"/>
       <c r="C12" s="6" t="s">
         <v>28</v>
       </c>
@@ -3360,7 +3684,7 @@
         <v>101</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F12" s="18" t="s">
         <v>70</v>
@@ -3373,32 +3697,32 @@
       </c>
       <c r="I12" s="5"/>
     </row>
-    <row r="13" spans="1:9" s="8" customFormat="1" ht="142.5">
-      <c r="A13" s="36"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="24" t="s">
+    <row r="13" spans="1:9" s="8" customFormat="1" ht="87.75">
+      <c r="A13" s="35"/>
+      <c r="B13" s="34"/>
+      <c r="C13" s="30" t="s">
         <v>107</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="30" t="s">
         <v>108</v>
       </c>
-      <c r="E13" s="24" t="s">
-        <v>125</v>
-      </c>
-      <c r="F13" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>12</v>
+      <c r="E13" s="30" t="s">
+        <v>139</v>
+      </c>
+      <c r="F13" s="38" t="s">
+        <v>147</v>
+      </c>
+      <c r="G13" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="H13" s="31" t="s">
+        <v>142</v>
       </c>
       <c r="I13" s="5"/>
     </row>
     <row r="14" spans="1:9" s="8" customFormat="1" ht="142.5">
-      <c r="A14" s="36"/>
-      <c r="B14" s="35"/>
+      <c r="A14" s="35"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="30" t="s">
         <v>106</v>
       </c>
@@ -3406,7 +3730,7 @@
         <v>109</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F14" s="31" t="s">
         <v>70</v>
@@ -3420,10 +3744,10 @@
       <c r="I14" s="5"/>
     </row>
     <row r="15" spans="1:9" s="8" customFormat="1" ht="71.25">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="34" t="s">
         <v>32</v>
       </c>
       <c r="C15" s="6" t="s">
@@ -3433,9 +3757,9 @@
         <v>110</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="F15" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="F15" s="32" t="s">
         <v>15</v>
       </c>
       <c r="G15" s="17" t="s">
@@ -3447,8 +3771,8 @@
       <c r="I15" s="5"/>
     </row>
     <row r="16" spans="1:9" s="8" customFormat="1" ht="71.25">
-      <c r="A16" s="36"/>
-      <c r="B16" s="35"/>
+      <c r="A16" s="35"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="6" t="s">
         <v>30</v>
       </c>
@@ -3456,9 +3780,9 @@
         <v>111</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>126</v>
-      </c>
-      <c r="F16" s="33"/>
+        <v>125</v>
+      </c>
+      <c r="F16" s="32"/>
       <c r="G16" s="17" t="s">
         <v>11</v>
       </c>
@@ -3468,8 +3792,8 @@
       <c r="I16" s="5"/>
     </row>
     <row r="17" spans="1:9" s="8" customFormat="1" ht="128.25">
-      <c r="A17" s="36"/>
-      <c r="B17" s="35"/>
+      <c r="A17" s="35"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="6" t="s">
         <v>33</v>
       </c>
@@ -3477,7 +3801,7 @@
         <v>71</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F17" s="19" t="s">
         <v>15</v>
@@ -3491,8 +3815,8 @@
       <c r="I17" s="5"/>
     </row>
     <row r="18" spans="1:9" s="8" customFormat="1" ht="128.25">
-      <c r="A18" s="36"/>
-      <c r="B18" s="35"/>
+      <c r="A18" s="35"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="6" t="s">
         <v>34</v>
       </c>
@@ -3500,7 +3824,7 @@
         <v>72</v>
       </c>
       <c r="E18" s="20" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F18" s="19" t="s">
         <v>15</v>
@@ -3514,18 +3838,18 @@
       <c r="I18" s="5"/>
     </row>
     <row r="19" spans="1:9" s="8" customFormat="1" ht="142.5">
-      <c r="A19" s="36"/>
-      <c r="B19" s="35"/>
+      <c r="A19" s="35"/>
+      <c r="B19" s="34"/>
       <c r="C19" s="6" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="F19" s="29" t="s">
+      <c r="E19" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" s="28" t="s">
         <v>15</v>
       </c>
       <c r="G19" s="20" t="s">
@@ -3537,18 +3861,18 @@
       <c r="I19" s="5"/>
     </row>
     <row r="20" spans="1:9" s="8" customFormat="1" ht="142.5">
-      <c r="A20" s="36"/>
-      <c r="B20" s="35"/>
+      <c r="A20" s="35"/>
+      <c r="B20" s="34"/>
       <c r="C20" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D20" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="F20" s="29" t="s">
+      <c r="E20" s="28" t="s">
+        <v>127</v>
+      </c>
+      <c r="F20" s="28" t="s">
         <v>15</v>
       </c>
       <c r="G20" s="20" t="s">
@@ -3560,10 +3884,10 @@
       <c r="I20" s="5"/>
     </row>
     <row r="21" spans="1:9" s="8" customFormat="1" ht="114">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="40" t="s">
         <v>41</v>
       </c>
       <c r="C21" s="6" t="s">
@@ -3572,8 +3896,8 @@
       <c r="D21" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="E21" s="29" t="s">
-        <v>129</v>
+      <c r="E21" s="28" t="s">
+        <v>128</v>
       </c>
       <c r="F21" s="21" t="s">
         <v>9</v>
@@ -3587,8 +3911,8 @@
       <c r="I21" s="5"/>
     </row>
     <row r="22" spans="1:9" s="8" customFormat="1" ht="114">
-      <c r="A22" s="36"/>
-      <c r="B22" s="35"/>
+      <c r="A22" s="40"/>
+      <c r="B22" s="40"/>
       <c r="C22" s="6" t="s">
         <v>39</v>
       </c>
@@ -3596,7 +3920,7 @@
         <v>113</v>
       </c>
       <c r="E22" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F22" s="6" t="s">
         <v>9</v>
@@ -3610,8 +3934,8 @@
       <c r="I22" s="5"/>
     </row>
     <row r="23" spans="1:9" s="8" customFormat="1" ht="142.5">
-      <c r="A23" s="36"/>
-      <c r="B23" s="35"/>
+      <c r="A23" s="40"/>
+      <c r="B23" s="40"/>
       <c r="C23" s="6" t="s">
         <v>40</v>
       </c>
@@ -3619,7 +3943,7 @@
         <v>114</v>
       </c>
       <c r="E23" s="20" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F23" s="20" t="s">
         <v>9</v>
@@ -3633,8 +3957,8 @@
       <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:9" s="8" customFormat="1" ht="99.75">
-      <c r="A24" s="36"/>
-      <c r="B24" s="35"/>
+      <c r="A24" s="40"/>
+      <c r="B24" s="40"/>
       <c r="C24" s="6" t="s">
         <v>42</v>
       </c>
@@ -3642,7 +3966,7 @@
         <v>115</v>
       </c>
       <c r="E24" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F24" s="20" t="s">
         <v>9</v>
@@ -3656,8 +3980,8 @@
       <c r="I24" s="5"/>
     </row>
     <row r="25" spans="1:9" s="8" customFormat="1" ht="128.25">
-      <c r="A25" s="36"/>
-      <c r="B25" s="35"/>
+      <c r="A25" s="40"/>
+      <c r="B25" s="40"/>
       <c r="C25" s="6" t="s">
         <v>43</v>
       </c>
@@ -3665,7 +3989,7 @@
         <v>116</v>
       </c>
       <c r="E25" s="20" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F25" s="20" t="s">
         <v>9</v>
@@ -3679,8 +4003,8 @@
       <c r="I25" s="5"/>
     </row>
     <row r="26" spans="1:9" s="8" customFormat="1" ht="114">
-      <c r="A26" s="36"/>
-      <c r="B26" s="35"/>
+      <c r="A26" s="40"/>
+      <c r="B26" s="40"/>
       <c r="C26" s="6" t="s">
         <v>44</v>
       </c>
@@ -3688,7 +4012,7 @@
         <v>77</v>
       </c>
       <c r="E26" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F26" s="20" t="s">
         <v>9</v>
@@ -3702,8 +4026,8 @@
       <c r="I26" s="5"/>
     </row>
     <row r="27" spans="1:9" s="8" customFormat="1" ht="114">
-      <c r="A27" s="36"/>
-      <c r="B27" s="35"/>
+      <c r="A27" s="40"/>
+      <c r="B27" s="40"/>
       <c r="C27" s="6" t="s">
         <v>45</v>
       </c>
@@ -3711,7 +4035,7 @@
         <v>78</v>
       </c>
       <c r="E27" s="20" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F27" s="20" t="s">
         <v>9</v>
@@ -3725,8 +4049,8 @@
       <c r="I27" s="5"/>
     </row>
     <row r="28" spans="1:9" s="8" customFormat="1" ht="99.75">
-      <c r="A28" s="36"/>
-      <c r="B28" s="35"/>
+      <c r="A28" s="40"/>
+      <c r="B28" s="40"/>
       <c r="C28" s="6" t="s">
         <v>46</v>
       </c>
@@ -3734,7 +4058,7 @@
         <v>79</v>
       </c>
       <c r="E28" s="20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F28" s="20" t="s">
         <v>9</v>
@@ -3748,8 +4072,8 @@
       <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9" s="8" customFormat="1" ht="128.25">
-      <c r="A29" s="36"/>
-      <c r="B29" s="35"/>
+      <c r="A29" s="40"/>
+      <c r="B29" s="40"/>
       <c r="C29" s="6" t="s">
         <v>57</v>
       </c>
@@ -3757,7 +4081,7 @@
         <v>117</v>
       </c>
       <c r="E29" s="22" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F29" s="20" t="s">
         <v>9</v>
@@ -3771,8 +4095,8 @@
       <c r="I29" s="5"/>
     </row>
     <row r="30" spans="1:9" s="8" customFormat="1" ht="85.5">
-      <c r="A30" s="36"/>
-      <c r="B30" s="35"/>
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
       <c r="C30" s="6" t="s">
         <v>47</v>
       </c>
@@ -3780,7 +4104,7 @@
         <v>80</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F30" s="20" t="s">
         <v>9</v>
@@ -3794,8 +4118,8 @@
       <c r="I30" s="5"/>
     </row>
     <row r="31" spans="1:9" s="8" customFormat="1" ht="114">
-      <c r="A31" s="36"/>
-      <c r="B31" s="35"/>
+      <c r="A31" s="40"/>
+      <c r="B31" s="40"/>
       <c r="C31" s="6" t="s">
         <v>48</v>
       </c>
@@ -3803,7 +4127,7 @@
         <v>75</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F31" s="21" t="s">
         <v>9</v>
@@ -3817,8 +4141,8 @@
       <c r="I31" s="5"/>
     </row>
     <row r="32" spans="1:9" s="8" customFormat="1" ht="99.75">
-      <c r="A32" s="36"/>
-      <c r="B32" s="35"/>
+      <c r="A32" s="40"/>
+      <c r="B32" s="40"/>
       <c r="C32" s="6" t="s">
         <v>49</v>
       </c>
@@ -3826,7 +4150,7 @@
         <v>64</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F32" s="21" t="s">
         <v>9</v>
@@ -3840,8 +4164,8 @@
       <c r="I32" s="5"/>
     </row>
     <row r="33" spans="1:9" s="8" customFormat="1" ht="99.75">
-      <c r="A33" s="36"/>
-      <c r="B33" s="35"/>
+      <c r="A33" s="40"/>
+      <c r="B33" s="40"/>
       <c r="C33" s="6" t="s">
         <v>50</v>
       </c>
@@ -3849,7 +4173,7 @@
         <v>63</v>
       </c>
       <c r="E33" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F33" s="21" t="s">
         <v>9</v>
@@ -3863,8 +4187,8 @@
       <c r="I33" s="5"/>
     </row>
     <row r="34" spans="1:9" s="8" customFormat="1" ht="99.75">
-      <c r="A34" s="36"/>
-      <c r="B34" s="35"/>
+      <c r="A34" s="40"/>
+      <c r="B34" s="40"/>
       <c r="C34" s="6" t="s">
         <v>51</v>
       </c>
@@ -3872,7 +4196,7 @@
         <v>62</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F34" s="21" t="s">
         <v>9</v>
@@ -3886,8 +4210,8 @@
       <c r="I34" s="5"/>
     </row>
     <row r="35" spans="1:9" s="8" customFormat="1" ht="114">
-      <c r="A35" s="36"/>
-      <c r="B35" s="35"/>
+      <c r="A35" s="40"/>
+      <c r="B35" s="40"/>
       <c r="C35" s="6" t="s">
         <v>52</v>
       </c>
@@ -3895,7 +4219,7 @@
         <v>76</v>
       </c>
       <c r="E35" s="16" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F35" s="21" t="s">
         <v>9</v>
@@ -3909,8 +4233,8 @@
       <c r="I35" s="5"/>
     </row>
     <row r="36" spans="1:9" s="8" customFormat="1" ht="42.75">
-      <c r="A36" s="36"/>
-      <c r="B36" s="35"/>
+      <c r="A36" s="40"/>
+      <c r="B36" s="40"/>
       <c r="C36" s="6" t="s">
         <v>53</v>
       </c>
@@ -3920,20 +4244,20 @@
       <c r="E36" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="F36" s="27" t="s">
+      <c r="F36" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="G36" s="27" t="s">
+      <c r="G36" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="H36" s="27" t="s">
+      <c r="H36" s="26" t="s">
         <v>14</v>
       </c>
       <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:9" s="8" customFormat="1" ht="44.25">
-      <c r="A37" s="36"/>
-      <c r="B37" s="35"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="6" t="s">
         <v>54</v>
       </c>
@@ -3948,213 +4272,237 @@
       <c r="H37" s="23"/>
       <c r="I37" s="5"/>
     </row>
-    <row r="38" spans="1:9" s="8" customFormat="1" ht="71.25">
-      <c r="A38" s="12" t="s">
+    <row r="38" spans="1:9" s="8" customFormat="1" ht="88.5">
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
+      <c r="C38" s="29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D38" s="29" t="s">
+        <v>149</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>151</v>
+      </c>
+      <c r="F38" s="38" t="s">
+        <v>150</v>
+      </c>
+      <c r="G38" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="H38" s="31" t="s">
+        <v>142</v>
+      </c>
+      <c r="I38" s="5"/>
+    </row>
+    <row r="39" spans="1:9" s="8" customFormat="1" ht="71.25">
+      <c r="A39" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B38" s="11"/>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11" t="s">
+      <c r="B39" s="11"/>
+      <c r="C39" s="11"/>
+      <c r="D39" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="E38" s="11"/>
-      <c r="F38" s="11"/>
-      <c r="G38" s="11"/>
-      <c r="H38" s="12"/>
-      <c r="I38" s="5"/>
-    </row>
-    <row r="39" spans="1:9" s="8" customFormat="1" ht="18" customHeight="1">
-      <c r="A39" s="36" t="s">
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="12"/>
+      <c r="I39" s="5"/>
+    </row>
+    <row r="40" spans="1:9" s="8" customFormat="1" ht="18" customHeight="1">
+      <c r="A40" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="B39" s="35" t="s">
+      <c r="B40" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C40" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="D39" s="28" t="s">
+      <c r="D40" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E39" s="35" t="s">
+      <c r="E40" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="F39" s="37" t="s">
+      <c r="F40" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="G39" s="37" t="s">
+      <c r="G40" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="H39" s="38" t="s">
+      <c r="H40" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="I39" s="5"/>
-    </row>
-    <row r="40" spans="1:9" s="8" customFormat="1">
-      <c r="A40" s="36"/>
-      <c r="B40" s="35"/>
-      <c r="C40" s="27" t="s">
+      <c r="I40" s="5"/>
+    </row>
+    <row r="41" spans="1:9" s="8" customFormat="1">
+      <c r="A41" s="35"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="D40" s="28" t="s">
+      <c r="D41" s="27" t="s">
         <v>91</v>
       </c>
-      <c r="E40" s="35"/>
-      <c r="F40" s="37"/>
-      <c r="G40" s="37"/>
-      <c r="H40" s="38"/>
-      <c r="I40" s="5"/>
-    </row>
-    <row r="41" spans="1:9" s="8" customFormat="1">
-      <c r="A41" s="36"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="27" t="s">
+      <c r="E41" s="34"/>
+      <c r="F41" s="36"/>
+      <c r="G41" s="36"/>
+      <c r="H41" s="37"/>
+      <c r="I41" s="5"/>
+    </row>
+    <row r="42" spans="1:9" s="8" customFormat="1">
+      <c r="A42" s="35"/>
+      <c r="B42" s="34"/>
+      <c r="C42" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="D41" s="28" t="s">
+      <c r="D42" s="27" t="s">
         <v>92</v>
       </c>
-      <c r="E41" s="35"/>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37"/>
-      <c r="H41" s="38"/>
-      <c r="I41" s="5"/>
-    </row>
-    <row r="42" spans="1:9" s="8" customFormat="1">
-      <c r="A42" s="36"/>
-      <c r="B42" s="35"/>
-      <c r="C42" s="27" t="s">
+      <c r="E42" s="34"/>
+      <c r="F42" s="36"/>
+      <c r="G42" s="36"/>
+      <c r="H42" s="37"/>
+      <c r="I42" s="5"/>
+    </row>
+    <row r="43" spans="1:9" s="8" customFormat="1">
+      <c r="A43" s="35"/>
+      <c r="B43" s="34"/>
+      <c r="C43" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="D42" s="28" t="s">
+      <c r="D43" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="E42" s="35"/>
-      <c r="F42" s="37"/>
-      <c r="G42" s="37"/>
-      <c r="H42" s="38"/>
-      <c r="I42" s="5"/>
-    </row>
-    <row r="43" spans="1:9" s="8" customFormat="1">
-      <c r="A43" s="36"/>
-      <c r="B43" s="35"/>
-      <c r="C43" s="27" t="s">
+      <c r="E43" s="34"/>
+      <c r="F43" s="36"/>
+      <c r="G43" s="36"/>
+      <c r="H43" s="37"/>
+      <c r="I43" s="5"/>
+    </row>
+    <row r="44" spans="1:9" s="8" customFormat="1">
+      <c r="A44" s="35"/>
+      <c r="B44" s="34"/>
+      <c r="C44" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="28" t="s">
+      <c r="D44" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="E43" s="35"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="37"/>
-      <c r="H43" s="38"/>
-      <c r="I43" s="5"/>
-    </row>
-    <row r="44" spans="1:9" s="8" customFormat="1">
-      <c r="A44" s="36"/>
-      <c r="B44" s="35"/>
-      <c r="C44" s="27" t="s">
+      <c r="E44" s="34"/>
+      <c r="F44" s="36"/>
+      <c r="G44" s="36"/>
+      <c r="H44" s="37"/>
+      <c r="I44" s="5"/>
+    </row>
+    <row r="45" spans="1:9" s="8" customFormat="1">
+      <c r="A45" s="35"/>
+      <c r="B45" s="34"/>
+      <c r="C45" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="D44" s="28" t="s">
+      <c r="D45" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="E44" s="35"/>
-      <c r="F44" s="37"/>
-      <c r="G44" s="37"/>
-      <c r="H44" s="38"/>
-      <c r="I44" s="5"/>
-    </row>
-    <row r="45" spans="1:9" s="8" customFormat="1">
-      <c r="A45" s="36"/>
-      <c r="B45" s="35"/>
-      <c r="C45" s="27" t="s">
+      <c r="E45" s="34"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="37"/>
+      <c r="I45" s="5"/>
+    </row>
+    <row r="46" spans="1:9" s="8" customFormat="1">
+      <c r="A46" s="35"/>
+      <c r="B46" s="34"/>
+      <c r="C46" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="D45" s="28" t="s">
+      <c r="D46" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="E45" s="35"/>
-      <c r="F45" s="37"/>
-      <c r="G45" s="37"/>
-      <c r="H45" s="38"/>
-      <c r="I45" s="5"/>
-    </row>
-    <row r="46" spans="1:9" s="8" customFormat="1">
-      <c r="A46" s="36"/>
-      <c r="B46" s="35"/>
-      <c r="C46" s="27" t="s">
+      <c r="E46" s="34"/>
+      <c r="F46" s="36"/>
+      <c r="G46" s="36"/>
+      <c r="H46" s="37"/>
+      <c r="I46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" s="8" customFormat="1">
+      <c r="A47" s="35"/>
+      <c r="B47" s="34"/>
+      <c r="C47" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="D46" s="28" t="s">
+      <c r="D47" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="35"/>
-      <c r="F46" s="37"/>
-      <c r="G46" s="37"/>
-      <c r="H46" s="38"/>
-      <c r="I46" s="5"/>
-    </row>
-    <row r="47" spans="1:9" s="8" customFormat="1">
-      <c r="A47" s="36"/>
-      <c r="B47" s="35"/>
-      <c r="C47" s="27" t="s">
+      <c r="E47" s="34"/>
+      <c r="F47" s="36"/>
+      <c r="G47" s="36"/>
+      <c r="H47" s="37"/>
+      <c r="I47" s="5"/>
+    </row>
+    <row r="48" spans="1:9" s="8" customFormat="1">
+      <c r="A48" s="35"/>
+      <c r="B48" s="34"/>
+      <c r="C48" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="D47" s="28" t="s">
+      <c r="D48" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="E47" s="35"/>
-      <c r="F47" s="37"/>
-      <c r="G47" s="37"/>
-      <c r="H47" s="38"/>
-      <c r="I47" s="5"/>
-    </row>
-    <row r="48" spans="1:9" s="8" customFormat="1">
-      <c r="A48" s="36"/>
-      <c r="B48" s="35"/>
-      <c r="C48" s="27" t="s">
+      <c r="E48" s="34"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="37"/>
+      <c r="I48" s="5"/>
+    </row>
+    <row r="49" spans="1:9" s="8" customFormat="1">
+      <c r="A49" s="35"/>
+      <c r="B49" s="34"/>
+      <c r="C49" s="26" t="s">
         <v>88</v>
       </c>
-      <c r="D48" s="28" t="s">
+      <c r="D49" s="27" t="s">
         <v>95</v>
       </c>
-      <c r="E48" s="35"/>
-      <c r="F48" s="37"/>
-      <c r="G48" s="37"/>
-      <c r="H48" s="38"/>
-      <c r="I48" s="5"/>
-    </row>
-    <row r="49" spans="1:9" s="10" customFormat="1">
-      <c r="A49" s="34" t="s">
+      <c r="E49" s="34"/>
+      <c r="F49" s="36"/>
+      <c r="G49" s="36"/>
+      <c r="H49" s="37"/>
+      <c r="I49" s="5"/>
+    </row>
+    <row r="50" spans="1:9" s="10" customFormat="1">
+      <c r="A50" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="B49" s="34"/>
-      <c r="C49" s="34"/>
-      <c r="D49" s="34"/>
-      <c r="E49" s="34"/>
-      <c r="F49" s="34"/>
-      <c r="G49" s="34"/>
-      <c r="H49" s="34"/>
-      <c r="I49" s="34"/>
+      <c r="B50" s="33"/>
+      <c r="C50" s="33"/>
+      <c r="D50" s="33"/>
+      <c r="E50" s="33"/>
+      <c r="F50" s="33"/>
+      <c r="G50" s="33"/>
+      <c r="H50" s="33"/>
+      <c r="I50" s="33"/>
     </row>
   </sheetData>
   <mergeCells count="14">
     <mergeCell ref="F15:F16"/>
-    <mergeCell ref="A49:I49"/>
+    <mergeCell ref="A50:I50"/>
     <mergeCell ref="B3:B14"/>
     <mergeCell ref="A3:A14"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="B15:B20"/>
-    <mergeCell ref="B39:B48"/>
-    <mergeCell ref="B21:B37"/>
-    <mergeCell ref="A21:A37"/>
-    <mergeCell ref="A39:A48"/>
-    <mergeCell ref="E39:E48"/>
-    <mergeCell ref="F39:F48"/>
-    <mergeCell ref="G39:G48"/>
-    <mergeCell ref="H39:H48"/>
+    <mergeCell ref="B40:B49"/>
+    <mergeCell ref="A40:A49"/>
+    <mergeCell ref="E40:E49"/>
+    <mergeCell ref="F40:F49"/>
+    <mergeCell ref="G40:G49"/>
+    <mergeCell ref="H40:H49"/>
+    <mergeCell ref="A21:A38"/>
+    <mergeCell ref="B21:B38"/>
   </mergeCells>
+  <phoneticPr fontId="10" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>